<commit_message>
ProcessorScalings ended and tested. Many little refactorizations (mainly working with Issues). A few bug fixes.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/06_upscale_almeria.xlsx
+++ b/backend_tests/z_input_files/v2/06_upscale_almeria.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="201">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -1188,7 +1188,7 @@
   </sheetPr>
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2212,8 +2212,8 @@
   </sheetPr>
   <dimension ref="A1:V54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R40" activeCellId="0" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3861,9 +3861,7 @@
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
-      <c r="R40" s="0" t="s">
-        <v>178</v>
-      </c>
+      <c r="R40" s="0"/>
       <c r="S40" s="0" t="n">
         <v>2015</v>
       </c>
@@ -3973,9 +3971,7 @@
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
-      <c r="R43" s="0" t="s">
-        <v>178</v>
-      </c>
+      <c r="R43" s="0"/>
       <c r="S43" s="0" t="n">
         <v>2015</v>
       </c>
@@ -4039,9 +4035,6 @@
       </c>
       <c r="M46" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="R46" s="0" t="s">
-        <v>178</v>
       </c>
       <c r="S46" s="0" t="n">
         <v>2015</v>

</xml_diff>